<commit_message>
PICARD-2383: Add musicbrainz_composerid to tag mapping and documentation
</commit_message>
<xml_diff>
--- a/_static/MusicBrainz_Picard_Tag_Map.xlsx
+++ b/_static/MusicBrainz_Picard_Tag_Map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="560">
   <si>
     <t>MusicBrainz Picard Tag Mapping</t>
   </si>
@@ -630,6 +630,18 @@
     <t>WM/ISRC</t>
   </si>
   <si>
+    <t>iTunes CDDB 1 [9]</t>
+  </si>
+  <si>
+    <t>itunes_cddb_1</t>
+  </si>
+  <si>
+    <t>iTunes_CDDB_1</t>
+  </si>
+  <si>
+    <t>----:com.apple.iTunes:iTunes_CDDB_1</t>
+  </si>
+  <si>
     <t>Language</t>
   </si>
   <si>
@@ -847,6 +859,24 @@
   </si>
   <si>
     <t>MusicBrainz/Artist Id</t>
+  </si>
+  <si>
+    <t>MusicBrainz Composer ID</t>
+  </si>
+  <si>
+    <t>musicbrainz_composerid</t>
+  </si>
+  <si>
+    <t>TXXX:MusicBrainz Composer Id</t>
+  </si>
+  <si>
+    <t>MUSICBRAINZ_COMPOSERID</t>
+  </si>
+  <si>
+    <t>----:com.apple.iTunes:MusicBrainz Composer Id</t>
+  </si>
+  <si>
+    <t>MusicBrainz/Composer Id</t>
   </si>
   <si>
     <t>MusicBrainz Disc ID</t>
@@ -2073,7 +2103,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -2939,68 +2969,68 @@
         <v>205</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>207</v>
-      </c>
       <c r="G35" s="4" t="s">
-        <v>208</v>
+        <v>15</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>209</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="E36" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="G37" s="4" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>15</v>
@@ -3008,25 +3038,25 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="E38" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>227</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>15</v>
@@ -3034,77 +3064,77 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>233</v>
-      </c>
       <c r="H39" s="4" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="E40" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>15</v>
@@ -3112,25 +3142,25 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="E42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>254</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>15</v>
@@ -3138,25 +3168,25 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>15</v>
@@ -3164,22 +3194,22 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>15</v>
@@ -3190,13 +3220,13 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>262</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>267</v>
@@ -3222,19 +3252,19 @@
         <v>270</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>273</v>
-      </c>
       <c r="G46" s="4" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>15</v>
@@ -3242,25 +3272,25 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="E47" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>280</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>15</v>
@@ -3268,25 +3298,25 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="E48" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>286</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>15</v>
@@ -3294,25 +3324,25 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="E49" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>292</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>15</v>
@@ -3320,25 +3350,25 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="E50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>296</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>15</v>
@@ -3346,25 +3376,25 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="E51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>304</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>15</v>
@@ -3372,25 +3402,25 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="E52" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>308</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>310</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>15</v>
@@ -3398,25 +3428,25 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="E53" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="G53" s="4" t="s">
         <v>314</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>316</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>15</v>
@@ -3424,25 +3454,25 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="E54" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="G54" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>322</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>15</v>
@@ -3450,25 +3480,25 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="E55" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="G55" s="4" t="s">
         <v>326</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>328</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>15</v>
@@ -3476,25 +3506,25 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="E56" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="G56" s="4" t="s">
         <v>332</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>15</v>
@@ -3502,25 +3532,25 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="E57" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="G57" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>15</v>
@@ -3528,25 +3558,25 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="E58" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="F58" s="4" t="s">
+      <c r="G58" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>15</v>
@@ -3554,25 +3584,25 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E59" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>15</v>
+        <v>349</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>349</v>
+        <v>15</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>15</v>
@@ -3589,16 +3619,16 @@
         <v>352</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>15</v>
+        <v>353</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>353</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>15</v>
+        <v>354</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>15</v>
@@ -3606,19 +3636,19 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>358</v>
+        <v>15</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>358</v>
+        <v>15</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>15</v>
@@ -3641,10 +3671,10 @@
         <v>362</v>
       </c>
       <c r="D62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>363</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>15</v>
@@ -3664,19 +3694,19 @@
         <v>366</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>15</v>
+        <v>367</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>15</v>
@@ -3684,25 +3714,25 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>373</v>
+        <v>15</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>15</v>
+        <v>374</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>15</v>
@@ -3710,25 +3740,25 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>376</v>
+        <v>15</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>15</v>
+        <v>378</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>15</v>
@@ -3736,22 +3766,22 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>15</v>
+        <v>381</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>15</v>
+        <v>382</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>15</v>
+        <v>383</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>379</v>
+        <v>15</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>15</v>
@@ -3762,28 +3792,28 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="3" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>382</v>
+        <v>15</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>383</v>
+        <v>15</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>385</v>
+        <v>15</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>386</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3794,19 +3824,19 @@
         <v>388</v>
       </c>
       <c r="C68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D68" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="G68" s="4" t="s">
-        <v>391</v>
+        <v>15</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>15</v>
@@ -3814,155 +3844,155 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="E69" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="F69" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="G69" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="H69" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="H69" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="E70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>404</v>
-      </c>
       <c r="H70" s="4" t="s">
-        <v>405</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="F71" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="G71" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>412</v>
-      </c>
       <c r="H71" s="4" t="s">
-        <v>413</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="G72" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="H72" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="G73" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="H73" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="E74" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="F74" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>430</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>434</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>15</v>
@@ -3970,25 +4000,25 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E75" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="G75" s="4" t="s">
         <v>437</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>438</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>15</v>
@@ -3996,25 +4026,25 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="E76" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="F76" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="E76" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="F76" s="4" t="s">
+      <c r="G76" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>443</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>15</v>
@@ -4164,13 +4194,13 @@
         <v>473</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>474</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>15</v>
@@ -4178,25 +4208,25 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D83" s="4" t="s">
-        <v>15</v>
+        <v>478</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>15</v>
+        <v>478</v>
       </c>
       <c r="F83" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="G83" s="4" t="s">
         <v>478</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>15</v>
@@ -4204,25 +4234,25 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="F84" s="4" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>15</v>
+        <v>485</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>15</v>
@@ -4230,22 +4260,22 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="3" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>484</v>
+        <v>15</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>485</v>
+        <v>15</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>485</v>
+        <v>15</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>15</v>
@@ -4256,25 +4286,25 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>489</v>
+        <v>15</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>490</v>
+        <v>15</v>
       </c>
       <c r="E86" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="F86" s="4" t="s">
-        <v>492</v>
-      </c>
       <c r="G86" s="4" t="s">
-        <v>493</v>
+        <v>15</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>15</v>
@@ -4282,25 +4312,25 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D87" s="4" t="s">
+      <c r="E87" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="E87" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="G87" s="4" t="s">
-        <v>497</v>
+        <v>15</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>15</v>
@@ -4308,25 +4338,25 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="C88" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="D88" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="E88" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="F88" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="G88" s="4" t="s">
         <v>503</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>15</v>
@@ -4340,123 +4370,123 @@
         <v>505</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>500</v>
+        <v>142</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>506</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>502</v>
+        <v>144</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>503</v>
+        <v>145</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>507</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>508</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="F90" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="F90" s="4" t="s">
-        <v>514</v>
-      </c>
       <c r="G90" s="4" t="s">
-        <v>513</v>
+        <v>15</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>515</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="E91" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="G91" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="H91" s="4" t="s">
         <v>518</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="F92" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="G92" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="H92" s="4" t="s">
         <v>525</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G92" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="H92" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="D93" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="E93" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="F93" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="G93" s="4" t="s">
         <v>531</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="G93" s="4" t="s">
-        <v>533</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>15</v>
@@ -4464,78 +4494,130 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="D94" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="E94" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="F94" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="H94" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="F94" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>539</v>
       </c>
+      <c r="C95" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="96" spans="1:8">
-      <c r="B96" s="5" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2">
-      <c r="B97" t="s">
-        <v>541</v>
+      <c r="A96" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" t="s">
-        <v>542</v>
+      <c r="B98" s="5" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" t="s">
-        <v>549</v>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>